<commit_message>
updated toy problems with accurate area
</commit_message>
<xml_diff>
--- a/ShapeLists/ToyLists.xlsx
+++ b/ShapeLists/ToyLists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alice K\Documents\Variable-Neighbourhood-Search\ShapeLists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD39241-3AF4-42BA-99DF-A9B3C9E29FD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEDF554-2314-4807-BC71-84D4F7988D3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,7 +387,7 @@
   <dimension ref="A1:K155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -440,19 +440,19 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>2520</v>
+        <v>1600</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
       </c>
       <c r="G3">
-        <v>25200</v>
+        <v>8000</v>
       </c>
       <c r="J3" t="s">
         <v>2</v>
       </c>
       <c r="K3" s="2">
-        <v>39908</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>